<commit_message>
[UPDATE] Tugas Minggu Ke 7 ditambah Fitur Cron Perminggu tambah data komoditas Tomat 500kg
</commit_message>
<xml_diff>
--- a/Source Code/latihan/tugas-minggu-7/assets/GeneratedDocument/Generated Production Komoditas Reports For Farm Pak Dengklek Created At-2023-01-16.xlsx
+++ b/Source Code/latihan/tugas-minggu-7/assets/GeneratedDocument/Generated Production Komoditas Reports For Farm Pak Dengklek Created At-2023-01-16.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="18">
   <si>
     <t>REPORT FILE GENERATED BY QUARKUS</t>
   </si>
@@ -53,6 +53,42 @@
   </si>
   <si>
     <t>UPDATED AT</t>
+  </si>
+  <si>
+    <t>cb155049-a59d-4c91-9454-a2fbac1c94a4</t>
+  </si>
+  <si>
+    <t>Bawang</t>
+  </si>
+  <si>
+    <t>2023-01-16T09:00:57.893924Z</t>
+  </si>
+  <si>
+    <t>00003944-c211-4828-84e0-8db3ceaa60fb</t>
+  </si>
+  <si>
+    <t>Brokoli</t>
+  </si>
+  <si>
+    <t>2023-01-16T09:01:05.133635Z</t>
+  </si>
+  <si>
+    <t>be6377de-e61e-4281-a6ea-9d20a5de0293</t>
+  </si>
+  <si>
+    <t>Wortel</t>
+  </si>
+  <si>
+    <t>2023-01-16T09:01:11.259338Z</t>
+  </si>
+  <si>
+    <t>7804bc9d-17f7-4293-9575-4fbd60f0fb8c</t>
+  </si>
+  <si>
+    <t>Jamur Trufle</t>
+  </si>
+  <si>
+    <t>2023-01-16T09:01:19.391102Z</t>
   </si>
 </sst>
 </file>
@@ -408,7 +444,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CECEC85C-72A7-4AB3-AF98-47886E3F9A4F}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -447,6 +483,74 @@
         <v>5</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" t="n">
+        <v>210.0</v>
+      </c>
+      <c r="D3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="n">
+        <v>310.0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" t="n">
+        <v>410.0</v>
+      </c>
+      <c r="D5" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="n">
+        <v>45.0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:J1"/>

</xml_diff>